<commit_message>
Update short read alternate analysis documentation with GO result column headers
</commit_message>
<xml_diff>
--- a/nanni_maize_2022/documentation/shrt_read_alt_analysis.xlsx
+++ b/nanni_maize_2022/documentation/shrt_read_alt_analysis.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\SHARE\McIntyre_Lab\maize_ozone_FINAL\2018\PacBio\documentation\github_documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\SHARE\McIntyre_Lab\maize_ozone_FINAL\2018\PacBio\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50DD04E7-36D6-40D4-BC03-B8CE3C997C98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A89B840-531B-4D3C-B0BD-67EA76C2ED3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1464" yWindow="1464" windowWidth="20736" windowHeight="10752" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2304" yWindow="2208" windowWidth="20736" windowHeight="10752" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="192">
   <si>
     <t>Analysis</t>
   </si>
@@ -533,6 +533,30 @@
 !!! Copied to SHARE: $PROJ/align_raw_reads_2_genomes/htseq_gene_counts/all_shrtRd_gene_htseq_count.tsv</t>
   </si>
   <si>
+    <t>Plot scatter plot of mean expression of coverage counts vs. RSEM</t>
+  </si>
+  <si>
+    <t>Plot scatter plot of RSEM  vs. Coverage counts TPM genes in maize
+** for genes NOT in assembled transcriptome and have evidence for PAV in Hoopes, et al. 2018
+!! 14877 genes with values present in assembled transcripts
+!! Count how many genes have values for cc and rs for at least one genotype
+==6681</t>
+  </si>
+  <si>
+    <t>## Must have matplotlib and seaborn so using TranD conda env
+export PATH=/TB14/TB14/conda_env/TranD/bin:$PATH
+$PROJ/2018/PacBio/scripts/plot_cvg_cnts_vs_rsem_scatter.py</t>
+  </si>
+  <si>
+    <t>$PROJ/2018/PacBio/scripts/run_plot_cvg_cnts_vs_rsem_scatter.sh</t>
+  </si>
+  <si>
+    <t>$PROJ/make_combination_flag_file/combined_tappas_output.csv</t>
+  </si>
+  <si>
+    <t>$PROJ/make_combination_flag_file/cvg_cnts_vs_rsem_mean_TPM_scatter.png</t>
+  </si>
+  <si>
     <t>Combine gene-level detection and analyzable flags with mean expression</t>
   </si>
   <si>
@@ -902,12 +926,96 @@
 Plot scatter plot comparing the mapped reads when mapped to B73 vs. Mo17 CAU
 Plot only 1-to-1 B73-Mo17 syntenic genes</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">!!! NOTE: ANALYSIS =
+            "rsemB73map" for the DE determined using assembled transcripts mapped to B73 and quantfied with RSEM,
+            "ccB73map" for the DE determined using B73 v4 reference transcripts quantified with genome alignments,
+            "ccB73mapBMo1to1" for the DE determined using the subset of genes from ccB73map that are 1-to-1 B73-Mo17 syntenic 
+            "ccMo17mapBMo1to1" for the DE determined using Mo17 Cau reference transcripts quantified with genome alignments 
+                        (and subset for genes that are 1-to-1 B83-Mo17 syntenic)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Column descriptions for comb_GO_gse_tappas_DE_${TYPE}_sig_terms.csv:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Term = GO term
+${ANALYSIS}_flag_DE_${GENO} = 1 if GO term is significant for genes DE in ${GENO}
+${ANALYSIS}_flag_DE_all = 1 if GO term is significant for genes DE in all 5 genotypes
+${ANALYSIS}_flag_DE_all_noB73 = 1 if GO term is significant for genes DE in C123, Hp301, Mo17, and NC338 and not DE in B73
+${ANALYSIS}_flag_B73Zero_restUp = 1 if GO term is significant for genes upregulated in elevated ozone in C123, Hp301, Mo17, and NC338 and unaffected in B73
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Column descriptions of ${TYPE}_identical_all_4_enrichments.csv:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">flag_DE_${GENO} = Number of analyses (0-4) where GO term is significant for genes DE in ${GENO}
+flag_DE_all = Number of analyses (0-4) where GO term is significant for genes DE in all 5 genotypes
+flag_DE_all_noB73 = Number of analyses (0-4) where GO term is significant for genes DE in C123, Hp301, Mo17, and NC338 and not DE in B73
+flag_B73Zero_restUp = Number of analyses (0-4) where GO term is significant for genes upregulated in elevated ozone in C123, Hp301, Mo17, and NC338 and unaffected in B73
+flag_DE_NC338_only = Number of analyses (0-4) where GO term is significant for genes DE in NC338 and not DE in the other 4 genotypes
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Columns descriptions of ${TYPE}_identical_${ANALYSIS_1}_${ANALYSIS_2}_enrichments.csv (pairwise comparisons of DE GO results):
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>** Flags are identical to ${TYPE}_identical_all_4_enrichments.csv, with the exception that these are pairwise comparisons, so the maximum number of analyses with the same significant go term is 2, if only 1 then the name of the one analysis (see names above) will be in the place of a number 1</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -972,8 +1080,21 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -984,6 +1105,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFDDDDDD"/>
         <bgColor rgb="FFCCFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1002,7 +1129,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1058,7 +1185,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1446,11 +1579,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J134"/>
+  <dimension ref="A1:J136"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1461,7 +1592,7 @@
     <col min="5" max="5" width="30.21875" customWidth="1"/>
     <col min="6" max="6" width="43.44140625" customWidth="1"/>
     <col min="7" max="7" width="51.6640625" customWidth="1"/>
-    <col min="8" max="8" width="104.88671875" customWidth="1"/>
+    <col min="8" max="8" width="115" customWidth="1"/>
     <col min="9" max="9" width="38.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1533,7 +1664,7 @@
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="C6" s="1" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -1583,22 +1714,22 @@
         <v>15</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -1607,19 +1738,19 @@
         <v>38</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -1628,19 +1759,19 @@
         <v>38</v>
       </c>
       <c r="B14" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="D14" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="C14" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>144</v>
-      </c>
       <c r="F14" s="7" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
     </row>
     <row r="15" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -1649,19 +1780,19 @@
         <v>38</v>
       </c>
       <c r="B16" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="F16" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="C16" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>153</v>
-      </c>
       <c r="G16" s="7" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
     </row>
     <row r="17" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -1670,19 +1801,19 @@
         <v>38</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
     </row>
     <row r="19" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -1691,10 +1822,10 @@
         <v>38</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
     </row>
     <row r="21" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -1808,7 +1939,7 @@
         <v>41</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="F30" s="7" t="s">
         <v>42</v>
@@ -2003,34 +2134,37 @@
         <v>38</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
     </row>
     <row r="49" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="50" spans="1:8" s="7" customFormat="1" ht="230.4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" s="7" customFormat="1" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A50" s="7" t="s">
         <v>38</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="F50" s="7" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="G50" s="7" t="s">
-        <v>182</v>
+        <v>188</v>
+      </c>
+      <c r="H50" s="21" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="51" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -2066,13 +2200,13 @@
         <v>90</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="D54" s="7" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="E54" s="7" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="F54" s="7" t="s">
         <v>91</v>
@@ -2184,73 +2318,73 @@
       </c>
     </row>
     <row r="63" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="64" spans="1:8" s="19" customFormat="1" ht="388.8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" s="19" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A64" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="B64" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="C64" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="D64" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="E64" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="F64" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="G64" s="19" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="66" spans="1:7" s="20" customFormat="1" ht="388.8" x14ac:dyDescent="0.3">
+      <c r="A66" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B64" s="19" t="s">
-        <v>166</v>
-      </c>
-      <c r="C64" s="19" t="s">
-        <v>167</v>
-      </c>
-      <c r="D64" s="19" t="s">
-        <v>168</v>
-      </c>
-      <c r="F64" s="19" t="s">
-        <v>169</v>
-      </c>
-      <c r="G64" s="19" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="66" spans="1:7" s="19" customFormat="1" ht="244.8" x14ac:dyDescent="0.3">
-      <c r="A66" s="19" t="s">
+      <c r="B66" s="20" t="s">
+        <v>172</v>
+      </c>
+      <c r="C66" s="20" t="s">
+        <v>173</v>
+      </c>
+      <c r="D66" s="20" t="s">
+        <v>174</v>
+      </c>
+      <c r="F66" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="G66" s="20" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="68" spans="1:7" s="20" customFormat="1" ht="244.8" x14ac:dyDescent="0.3">
+      <c r="A68" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B66" s="19" t="s">
-        <v>171</v>
-      </c>
-      <c r="C66" s="19" t="s">
-        <v>175</v>
-      </c>
-      <c r="D66" s="19" t="s">
-        <v>172</v>
-      </c>
-      <c r="F66" s="19" t="s">
-        <v>173</v>
-      </c>
-      <c r="G66" s="19" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="68" spans="1:7" s="7" customFormat="1" ht="259.2" x14ac:dyDescent="0.3">
-      <c r="A68" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="B68" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="C68" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="D68" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="E68" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="F68" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="G68" s="7" t="s">
-        <v>123</v>
+      <c r="B68" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="C68" s="20" t="s">
+        <v>181</v>
+      </c>
+      <c r="D68" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="F68" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="G68" s="20" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="69" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="70" spans="1:7" s="7" customFormat="1" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" s="7" customFormat="1" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A70" s="7" t="s">
         <v>38</v>
       </c>
@@ -2264,89 +2398,89 @@
         <v>126</v>
       </c>
       <c r="E70" s="7" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="F70" s="7" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="G70" s="7" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="71" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="72" spans="1:7" s="7" customFormat="1" ht="144" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7" s="7" customFormat="1" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A72" s="7" t="s">
         <v>38</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C72" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="D72" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="E72" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="F72" s="7" t="s">
         <v>129</v>
-      </c>
-      <c r="D72" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="E72" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="F72" s="7" t="s">
-        <v>132</v>
       </c>
       <c r="G72" s="7" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="73" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="74" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="75" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="73" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="74" spans="1:7" s="7" customFormat="1" ht="144" x14ac:dyDescent="0.3">
+      <c r="A74" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B74" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="C74" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="D74" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="E74" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="F74" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="G74" s="7" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="76" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="77" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="78" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="78" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="79" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="80" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="80" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="81" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="82" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="83" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="84" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="85" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="86" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="83" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="84" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="85" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="86" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="87" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="88" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="89" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="90" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B90" s="3"/>
-      <c r="C90" s="11"/>
-      <c r="D90" s="11"/>
-      <c r="E90" s="3"/>
-      <c r="F90" s="12"/>
-      <c r="G90" s="12"/>
-      <c r="H90" s="12"/>
-      <c r="I90" s="12"/>
-    </row>
-    <row r="92" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="3"/>
+    <row r="89" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="90" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="91" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="92" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B92" s="3"/>
       <c r="C92" s="11"/>
       <c r="D92" s="11"/>
       <c r="E92" s="3"/>
-      <c r="F92" s="3"/>
-      <c r="G92" s="3"/>
-      <c r="H92" s="3"/>
-      <c r="I92" s="13"/>
-      <c r="J92" s="13"/>
-    </row>
-    <row r="93" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="3"/>
-      <c r="B93" s="3"/>
-      <c r="C93" s="11"/>
-      <c r="D93" s="11"/>
-      <c r="E93" s="3"/>
-      <c r="F93" s="3"/>
-      <c r="G93" s="3"/>
-      <c r="H93" s="3"/>
-      <c r="I93" s="13"/>
-      <c r="J93" s="13"/>
+      <c r="F92" s="12"/>
+      <c r="G92" s="12"/>
+      <c r="H92" s="12"/>
+      <c r="I92" s="12"/>
     </row>
     <row r="94" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A94" s="3"/>
@@ -2396,41 +2530,41 @@
       <c r="I97" s="13"/>
       <c r="J97" s="13"/>
     </row>
-    <row r="98" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="99" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="100" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="15"/>
-      <c r="B100" s="15"/>
-      <c r="C100" s="16"/>
-      <c r="D100" s="16"/>
-      <c r="E100" s="15"/>
-      <c r="F100" s="15"/>
-      <c r="G100" s="15"/>
-      <c r="H100" s="15"/>
-    </row>
-    <row r="101" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="3"/>
-      <c r="B101" s="3"/>
-      <c r="C101" s="11"/>
-      <c r="D101" s="11"/>
-      <c r="E101" s="3"/>
-      <c r="F101" s="3"/>
-      <c r="G101" s="3"/>
-      <c r="H101" s="3"/>
-      <c r="I101" s="13"/>
-      <c r="J101" s="13"/>
-    </row>
-    <row r="102" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="3"/>
-      <c r="B102" s="3"/>
-      <c r="C102" s="11"/>
-      <c r="D102" s="11"/>
-      <c r="E102" s="11"/>
-      <c r="F102" s="3"/>
-      <c r="G102" s="3"/>
-      <c r="H102" s="3"/>
-      <c r="I102" s="13"/>
-      <c r="J102" s="13"/>
+    <row r="98" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="3"/>
+      <c r="B98" s="3"/>
+      <c r="C98" s="11"/>
+      <c r="D98" s="11"/>
+      <c r="E98" s="3"/>
+      <c r="F98" s="3"/>
+      <c r="G98" s="3"/>
+      <c r="H98" s="3"/>
+      <c r="I98" s="13"/>
+      <c r="J98" s="13"/>
+    </row>
+    <row r="99" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A99" s="3"/>
+      <c r="B99" s="3"/>
+      <c r="C99" s="11"/>
+      <c r="D99" s="11"/>
+      <c r="E99" s="3"/>
+      <c r="F99" s="3"/>
+      <c r="G99" s="3"/>
+      <c r="H99" s="3"/>
+      <c r="I99" s="13"/>
+      <c r="J99" s="13"/>
+    </row>
+    <row r="100" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="101" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="102" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="15"/>
+      <c r="B102" s="15"/>
+      <c r="C102" s="16"/>
+      <c r="D102" s="16"/>
+      <c r="E102" s="15"/>
+      <c r="F102" s="15"/>
+      <c r="G102" s="15"/>
+      <c r="H102" s="15"/>
     </row>
     <row r="103" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A103" s="3"/>
@@ -2444,49 +2578,49 @@
       <c r="I103" s="13"/>
       <c r="J103" s="13"/>
     </row>
-    <row r="104" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="15"/>
-      <c r="B104" s="15"/>
-      <c r="C104" s="16"/>
-      <c r="D104" s="16"/>
-      <c r="E104" s="15"/>
-      <c r="F104" s="15"/>
-      <c r="G104" s="15"/>
-      <c r="H104" s="15"/>
-    </row>
-    <row r="105" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="15"/>
-      <c r="B105" s="15"/>
-      <c r="C105" s="16"/>
-      <c r="D105" s="16"/>
-      <c r="E105" s="15"/>
-      <c r="F105" s="15"/>
-      <c r="G105" s="15"/>
-      <c r="H105" s="15"/>
-    </row>
-    <row r="106" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="3"/>
-      <c r="B106" s="3"/>
-      <c r="C106" s="11"/>
-      <c r="D106" s="11"/>
-      <c r="E106" s="11"/>
-      <c r="F106" s="3"/>
-      <c r="G106" s="3"/>
-      <c r="H106" s="3"/>
-      <c r="I106" s="13"/>
-      <c r="J106" s="13"/>
-    </row>
-    <row r="107" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="3"/>
-      <c r="B107" s="3"/>
-      <c r="C107" s="11"/>
-      <c r="D107" s="11"/>
-      <c r="E107" s="11"/>
-      <c r="F107" s="3"/>
-      <c r="G107" s="3"/>
-      <c r="H107" s="3"/>
-      <c r="I107" s="13"/>
-      <c r="J107" s="13"/>
+    <row r="104" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A104" s="3"/>
+      <c r="B104" s="3"/>
+      <c r="C104" s="11"/>
+      <c r="D104" s="11"/>
+      <c r="E104" s="11"/>
+      <c r="F104" s="3"/>
+      <c r="G104" s="3"/>
+      <c r="H104" s="3"/>
+      <c r="I104" s="13"/>
+      <c r="J104" s="13"/>
+    </row>
+    <row r="105" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="3"/>
+      <c r="B105" s="3"/>
+      <c r="C105" s="11"/>
+      <c r="D105" s="11"/>
+      <c r="E105" s="3"/>
+      <c r="F105" s="3"/>
+      <c r="G105" s="3"/>
+      <c r="H105" s="3"/>
+      <c r="I105" s="13"/>
+      <c r="J105" s="13"/>
+    </row>
+    <row r="106" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A106" s="15"/>
+      <c r="B106" s="15"/>
+      <c r="C106" s="16"/>
+      <c r="D106" s="16"/>
+      <c r="E106" s="15"/>
+      <c r="F106" s="15"/>
+      <c r="G106" s="15"/>
+      <c r="H106" s="15"/>
+    </row>
+    <row r="107" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A107" s="15"/>
+      <c r="B107" s="15"/>
+      <c r="C107" s="16"/>
+      <c r="D107" s="16"/>
+      <c r="E107" s="15"/>
+      <c r="F107" s="15"/>
+      <c r="G107" s="15"/>
+      <c r="H107" s="15"/>
     </row>
     <row r="108" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A108" s="3"/>
@@ -2536,24 +2670,24 @@
       <c r="I111" s="13"/>
       <c r="J111" s="13"/>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A112" s="7"/>
+    <row r="112" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A112" s="3"/>
       <c r="B112" s="3"/>
-      <c r="C112" s="15"/>
-      <c r="D112" s="15"/>
-      <c r="E112" s="15"/>
-      <c r="F112" s="11"/>
-      <c r="G112" s="15"/>
+      <c r="C112" s="11"/>
+      <c r="D112" s="11"/>
+      <c r="E112" s="11"/>
+      <c r="F112" s="3"/>
+      <c r="G112" s="3"/>
       <c r="H112" s="3"/>
       <c r="I112" s="13"/>
       <c r="J112" s="13"/>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A113" s="3"/>
       <c r="B113" s="3"/>
-      <c r="C113" s="1"/>
-      <c r="D113" s="1"/>
-      <c r="E113" s="1"/>
+      <c r="C113" s="11"/>
+      <c r="D113" s="11"/>
+      <c r="E113" s="11"/>
       <c r="F113" s="3"/>
       <c r="G113" s="3"/>
       <c r="H113" s="3"/>
@@ -2566,8 +2700,8 @@
       <c r="C114" s="15"/>
       <c r="D114" s="15"/>
       <c r="E114" s="15"/>
-      <c r="F114" s="3"/>
-      <c r="G114" s="3"/>
+      <c r="F114" s="11"/>
+      <c r="G114" s="15"/>
       <c r="H114" s="3"/>
       <c r="I114" s="13"/>
       <c r="J114" s="13"/>
@@ -2586,23 +2720,27 @@
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A116" s="7"/>
-      <c r="B116" s="15"/>
+      <c r="B116" s="3"/>
       <c r="C116" s="15"/>
       <c r="D116" s="15"/>
       <c r="E116" s="15"/>
-      <c r="F116" s="15"/>
-      <c r="G116" s="15"/>
-      <c r="H116" s="15"/>
+      <c r="F116" s="3"/>
+      <c r="G116" s="3"/>
+      <c r="H116" s="3"/>
+      <c r="I116" s="13"/>
+      <c r="J116" s="13"/>
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A117" s="7"/>
-      <c r="B117" s="15"/>
-      <c r="C117" s="15"/>
-      <c r="D117" s="15"/>
-      <c r="E117" s="15"/>
-      <c r="F117" s="15"/>
-      <c r="G117" s="15"/>
-      <c r="H117" s="15"/>
+      <c r="A117" s="3"/>
+      <c r="B117" s="3"/>
+      <c r="C117" s="1"/>
+      <c r="D117" s="1"/>
+      <c r="E117" s="1"/>
+      <c r="F117" s="3"/>
+      <c r="G117" s="3"/>
+      <c r="H117" s="3"/>
+      <c r="I117" s="13"/>
+      <c r="J117" s="13"/>
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A118" s="7"/>
@@ -2615,63 +2753,83 @@
       <c r="H118" s="15"/>
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A119" s="4"/>
-      <c r="B119" s="1"/>
-      <c r="C119" s="1"/>
-      <c r="D119" s="1"/>
-      <c r="E119" s="1"/>
-      <c r="F119" s="1"/>
-      <c r="G119" s="1"/>
-      <c r="H119" s="1"/>
-    </row>
-    <row r="120" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A120" s="3"/>
-      <c r="B120" s="3"/>
-      <c r="C120" s="11"/>
-      <c r="D120" s="11"/>
-      <c r="E120" s="11"/>
-      <c r="F120" s="3"/>
-      <c r="G120" s="3"/>
-      <c r="H120" s="3"/>
-      <c r="I120" s="13"/>
-      <c r="J120" s="13"/>
-    </row>
-    <row r="121" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="122" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="123" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="124" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="125" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+      <c r="A119" s="7"/>
+      <c r="B119" s="15"/>
+      <c r="C119" s="15"/>
+      <c r="D119" s="15"/>
+      <c r="E119" s="15"/>
+      <c r="F119" s="15"/>
+      <c r="G119" s="15"/>
+      <c r="H119" s="15"/>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A120" s="7"/>
+      <c r="B120" s="15"/>
+      <c r="C120" s="15"/>
+      <c r="D120" s="15"/>
+      <c r="E120" s="15"/>
+      <c r="F120" s="15"/>
+      <c r="G120" s="15"/>
+      <c r="H120" s="15"/>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A121" s="4"/>
+      <c r="B121" s="1"/>
+      <c r="C121" s="1"/>
+      <c r="D121" s="1"/>
+      <c r="E121" s="1"/>
+      <c r="F121" s="1"/>
+      <c r="G121" s="1"/>
+      <c r="H121" s="1"/>
+    </row>
+    <row r="122" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A122" s="3"/>
+      <c r="B122" s="3"/>
+      <c r="C122" s="11"/>
+      <c r="D122" s="11"/>
+      <c r="E122" s="11"/>
+      <c r="F122" s="3"/>
+      <c r="G122" s="3"/>
+      <c r="H122" s="3"/>
+      <c r="I122" s="13"/>
+      <c r="J122" s="13"/>
+    </row>
+    <row r="123" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="124" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="125" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="126" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A127" s="7"/>
-      <c r="B127" s="15"/>
-      <c r="C127" s="15"/>
-      <c r="D127" s="15"/>
-      <c r="E127" s="7"/>
-      <c r="F127" s="15"/>
-      <c r="G127" s="15"/>
-      <c r="H127" s="15"/>
-    </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A128" s="7"/>
-      <c r="B128" s="15"/>
-      <c r="C128" s="15"/>
-      <c r="D128" s="15"/>
-      <c r="E128" s="7"/>
-      <c r="F128" s="15"/>
-      <c r="G128" s="15"/>
-      <c r="H128" s="15"/>
-    </row>
-    <row r="129" spans="5:5" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="130" spans="5:5" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="131" spans="5:5" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="132" spans="5:5" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="133" spans="5:5" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="134" spans="5:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="E134" s="7"/>
+    <row r="127" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="128" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A129" s="7"/>
+      <c r="B129" s="15"/>
+      <c r="C129" s="15"/>
+      <c r="D129" s="15"/>
+      <c r="E129" s="7"/>
+      <c r="F129" s="15"/>
+      <c r="G129" s="15"/>
+      <c r="H129" s="15"/>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A130" s="7"/>
+      <c r="B130" s="15"/>
+      <c r="C130" s="15"/>
+      <c r="D130" s="15"/>
+      <c r="E130" s="7"/>
+      <c r="F130" s="15"/>
+      <c r="G130" s="15"/>
+      <c r="H130" s="15"/>
+    </row>
+    <row r="131" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="132" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="133" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="134" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="135" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="136" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E136" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>